<commit_message>
updated name of the datasets
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/Map_of_donors_Concluded_Final_funding.xlsx
+++ b/Simple_XLS_Importer/data/Map_of_donors_Concluded_Final_funding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="2355" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="151">
   <si>
     <t>ISO3</t>
   </si>
@@ -423,6 +423,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>: In the original dataset each observation was a project. In order to ingest it in the LB we aggregated all projects by target country ("country_names")</t>
     </r>
@@ -436,6 +437,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Where a single project was implemented in multiple countries the same share of total foundings have been allocated to each country included in the project as a beneficiary</t>
     </r>
@@ -448,6 +450,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>: for the generation of "N° of target countries for each project" column: NA when "country_names"="Global relevance"; No value when "country_names" is missing</t>
     </r>
@@ -460,6 +463,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>: Only project with full information on "activity_start_date", "actiity_end_date" will be included in the dataset for ingestion; Project without full info on fundings have not been deleted.</t>
     </r>
@@ -472,6 +476,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>: Project ID's have been added to the original file, so that changes from the original dataset to the intermediate and to the final one can be tracked</t>
     </r>
@@ -515,6 +520,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>: Looking at "activity_end_dt" we differenciated between on-going and concluded projects; Project are labelled "concluded" if "activity_end_date" is equal or smaller than Dec_2015</t>
     </r>
@@ -527,6 +533,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>: All projects still in operation in Jan 2016; If a project ended in January 2016 will be considered "ongoing", while a project ended in Dec 2015 is concluded</t>
     </r>
@@ -536,9 +543,6 @@
   </si>
   <si>
     <t>DP</t>
-  </si>
-  <si>
-    <t>MOD-1</t>
   </si>
   <si>
     <t>MOD-C-F</t>
@@ -551,7 +555,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -566,38 +570,49 @@
       <i/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -669,16 +684,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1021,7 +1036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -2185,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2215,7 +2230,7 @@
         <v>142</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2246,56 +2261,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.1" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="16" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="15"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
@@ -2538,18 +2553,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
updated the name of the dataset
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/Map_of_donors_Concluded_Final_funding.xlsx
+++ b/Simple_XLS_Importer/data/Map_of_donors_Concluded_Final_funding.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="152">
   <si>
     <t>ISO3</t>
   </si>
@@ -546,6 +546,9 @@
   </si>
   <si>
     <t>MOD-C-F</t>
+  </si>
+  <si>
+    <t>MOD</t>
   </si>
 </sst>
 </file>
@@ -684,16 +687,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2201,7 +2204,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2222,7 +2225,7 @@
         <v>141</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2261,56 +2264,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.1" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
@@ -2553,18 +2556,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>